<commit_message>
minor edit to cannonrange (cursor position)
</commit_message>
<xml_diff>
--- a/data/cannon_range.xlsx
+++ b/data/cannon_range.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{870643D6-2908-4E39-A70E-93841D9BBD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{461BE14D-31E3-4C24-8A77-E72F57708B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{E0B0BD53-29FB-4041-980E-7A118E355A61}"/>
   </bookViews>
@@ -464,9 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38A76A0-6CE7-4157-B47C-9713439C6F05}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>